<commit_message>
add university chance function
</commit_message>
<xml_diff>
--- a/Planning/progress.xlsx
+++ b/Planning/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\RandomCreation\project\DSELife\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBBAD9D-A938-4A1D-8302-99C5BDF958A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760949A3-0938-4627-AAA0-9EC78442C331}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{46DBBE32-2521-49FB-B55D-2654E6CA81D1}"/>
   </bookViews>
@@ -270,7 +270,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -324,6 +324,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -639,15 +642,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35778905-F7DA-47E9-8A70-E68EC8D85338}">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G7" sqref="G7:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -673,7 +676,7 @@
       <c r="Q1" s="16"/>
       <c r="R1" s="17"/>
     </row>
-    <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -682,6 +685,14 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="6"/>
+      <c r="G2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="4"/>
       <c r="M2" s="2" t="s">
         <v>14</v>
       </c>
@@ -691,7 +702,7 @@
       <c r="Q2" s="9"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
@@ -715,7 +726,7 @@
       <c r="Q3" s="9"/>
       <c r="R3" s="4"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -730,16 +741,8 @@
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
       <c r="L4" s="4"/>
-      <c r="M4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="4"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -763,7 +766,7 @@
       <c r="Q5" s="9"/>
       <c r="R5" s="4"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
@@ -787,7 +790,7 @@
       <c r="Q6" s="9"/>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>13</v>
       </c>
@@ -811,7 +814,7 @@
       <c r="Q7" s="9"/>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G8" s="2"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -826,8 +829,9 @@
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
       <c r="R8" s="9"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S8" s="18"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
@@ -849,7 +853,7 @@
       <c r="Q9" s="9"/>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -871,7 +875,7 @@
       <c r="Q10" s="9"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -893,7 +897,7 @@
       <c r="Q11" s="9"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
@@ -915,7 +919,7 @@
       <c r="Q12" s="9"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G13" s="2"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
@@ -929,7 +933,7 @@
       <c r="Q13" s="9"/>
       <c r="R13" s="4"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>9</v>
       </c>
@@ -951,7 +955,7 @@
       <c r="Q14" s="9"/>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -973,7 +977,7 @@
       <c r="Q15" s="3"/>
       <c r="R15" s="4"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
@@ -995,7 +999,7 @@
     <mergeCell ref="A12:F12"/>
     <mergeCell ref="M2:R2"/>
     <mergeCell ref="M3:R3"/>
-    <mergeCell ref="M4:R4"/>
+    <mergeCell ref="G2:L2"/>
     <mergeCell ref="M5:R5"/>
     <mergeCell ref="M6:R6"/>
     <mergeCell ref="M7:R7"/>

</xml_diff>

<commit_message>
add money useup status label
</commit_message>
<xml_diff>
--- a/Planning/progress.xlsx
+++ b/Planning/progress.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\RandomCreation\HKDSE\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\RandomCreation\project\DSELife\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41B36DB-40CD-44B4-AABC-1D29DF419A07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161A19A5-BD7D-4754-8964-5063DEE9A4F5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{46DBBE32-2521-49FB-B55D-2654E6CA81D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{46DBBE32-2521-49FB-B55D-2654E6CA81D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>add whole day scheldude</t>
+    <t>add whole day scheldude(Layered lane)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -124,18 +124,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -144,10 +144,16 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -270,7 +276,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -280,6 +286,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -289,6 +313,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -298,34 +331,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -645,344 +654,362 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:L2"/>
+      <selection activeCell="G14" sqref="G14:L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" thickBot="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="3" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="3" t="s">
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="5"/>
-    </row>
-    <row r="2" spans="1:19" ht="15" thickBot="1">
-      <c r="A2" s="17" t="s">
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="11"/>
+    </row>
+    <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="9" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="5"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
+      <c r="M3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="5"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="5"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="5"/>
+      <c r="S8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="5"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="5"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="5"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="5"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="13"/>
-    </row>
-    <row r="3" spans="1:19">
-      <c r="A3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="13"/>
-    </row>
-    <row r="4" spans="1:19">
-      <c r="A4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="13"/>
-    </row>
-    <row r="5" spans="1:19">
-      <c r="A5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="13"/>
-    </row>
-    <row r="6" spans="1:19">
-      <c r="A6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="13"/>
-    </row>
-    <row r="7" spans="1:19">
-      <c r="A7" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="9" t="s">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="5"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="5"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="5"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="13"/>
-    </row>
-    <row r="8" spans="1:19">
-      <c r="A8" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="2"/>
-    </row>
-    <row r="9" spans="1:19">
-      <c r="A9" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="13"/>
-    </row>
-    <row r="10" spans="1:19">
-      <c r="A10" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="13"/>
-    </row>
-    <row r="11" spans="1:19">
-      <c r="A11" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="13"/>
-    </row>
-    <row r="12" spans="1:19">
-      <c r="A12" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="13"/>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="G13" s="9"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="13"/>
-    </row>
-    <row r="14" spans="1:19">
-      <c r="A14" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="13"/>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="A15" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="13"/>
-    </row>
-    <row r="16" spans="1:19">
-      <c r="F16" s="1"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="5"/>
       <c r="G16" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="42">
+  <mergeCells count="41">
+    <mergeCell ref="M1:R1"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="G2:L2"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="G4:L4"/>
+    <mergeCell ref="G5:L5"/>
+    <mergeCell ref="G6:L6"/>
+    <mergeCell ref="M2:R2"/>
+    <mergeCell ref="M3:R3"/>
+    <mergeCell ref="M5:R5"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:L1"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="G15:L15"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="G8:L8"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="G9:L9"/>
+    <mergeCell ref="G10:L10"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="G12:L12"/>
     <mergeCell ref="M15:R15"/>
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="A4:F4"/>
@@ -999,32 +1026,6 @@
     <mergeCell ref="G13:L13"/>
     <mergeCell ref="G14:L14"/>
     <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:L1"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="G15:L15"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="G8:L8"/>
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="G9:L9"/>
-    <mergeCell ref="G10:L10"/>
-    <mergeCell ref="G11:L11"/>
-    <mergeCell ref="G12:L12"/>
-    <mergeCell ref="G3:L3"/>
-    <mergeCell ref="M1:R1"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="M8:R8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="G4:L4"/>
-    <mergeCell ref="G5:L5"/>
-    <mergeCell ref="G6:L6"/>
-    <mergeCell ref="M2:R2"/>
-    <mergeCell ref="M3:R3"/>
-    <mergeCell ref="M5:R5"/>
-    <mergeCell ref="G2:L2"/>
-    <mergeCell ref="M7:R7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>